<commit_message>
update front and back
</commit_message>
<xml_diff>
--- a/project-folder/data/challenges.xlsx
+++ b/project-folder/data/challenges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/545051a8d7303bb2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\github\around_ch\project-folder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C276CA32-D4CC-4EC5-844E-05035B7988E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AB376B-3DB5-474B-A11A-C363C68423D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="5780" windowWidth="19080" windowHeight="16660" xr2:uid="{6C5A2459-C472-46C9-B1BC-BCC00E567CF2}"/>
+    <workbookView xWindow="18540" yWindow="3560" windowWidth="19080" windowHeight="16660" xr2:uid="{6C5A2459-C472-46C9-B1BC-BCC00E567CF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>art_der_challenge</t>
   </si>
@@ -47,28 +47,13 @@
     <t>geojson_key</t>
   </si>
   <si>
-    <t>genfersee</t>
-  </si>
-  <si>
-    <t>bielersee</t>
-  </si>
-  <si>
     <t>Genferseeumrundung</t>
   </si>
   <si>
     <t>Bielerseeumrundung</t>
   </si>
   <si>
-    <t>Murtenseeumrundung</t>
-  </si>
-  <si>
     <t>Neuenburgerseeumrundung</t>
-  </si>
-  <si>
-    <t>murtensee</t>
-  </si>
-  <si>
-    <t>neuenburgersee</t>
   </si>
 </sst>
 </file>
@@ -90,7 +75,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color rgb="FF101010"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -140,7 +126,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -475,17 +463,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575D18FD-C522-49EA-A191-D8B369547A7C}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.81640625" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -501,10 +489,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>199884</v>
+        <v>190980</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -512,10 +500,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>55602</v>
+        <v>516500</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -523,27 +511,17 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>23611</v>
+        <v>983300</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>119556</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>